<commit_message>
continue building out generic method for OES tables
</commit_message>
<xml_diff>
--- a/INPUT-FILES/self-agestrat-rawToSS.xlsx
+++ b/INPUT-FILES/self-agestrat-rawToSS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dherzberg/Desktop/R/DP4-R/DOCUMENTATION/DEMO-INPUT-TABLES/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dherzberg/Desktop/R/OES-INPUT-TABLES/INPUT-FILES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7D3D5E-5C63-7646-A8DD-F3DEFB664762}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF3D1AC-8873-8C43-9110-4D232956A18B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="1" xr2:uid="{C9FF4BE8-38E8-4C4A-AC74-EE9A69DC62CF}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="17540" activeTab="1" xr2:uid="{C9FF4BE8-38E8-4C4A-AC74-EE9A69DC62CF}"/>
   </bookViews>
   <sheets>
     <sheet name="060" sheetId="1" r:id="rId1"/>
@@ -418,10 +418,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C2">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -429,10 +429,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -440,10 +440,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C4">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -451,10 +451,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C5">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -462,10 +462,10 @@
         <v>5</v>
       </c>
       <c r="B6">
+        <v>112</v>
+      </c>
+      <c r="C6">
         <v>111</v>
-      </c>
-      <c r="C6">
-        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -478,7 +478,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -499,10 +499,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C2">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -510,10 +510,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C3">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -521,10 +521,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C4">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -532,10 +532,10 @@
         <v>4</v>
       </c>
       <c r="B5">
+        <v>105</v>
+      </c>
+      <c r="C5">
         <v>107</v>
-      </c>
-      <c r="C5">
-        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -543,10 +543,10 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C6">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>